<commit_message>
Court Order Outfile checkin
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/TestOutPutResultFolder/201819 Payroll Court order and Student Loan Test result.xlsx
+++ b/Salesforce_Core_Framework/TestOutPutResultFolder/201819 Payroll Court order and Student Loan Test result.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Automation_TestResults\Payroll_CourtOrderScenarios 201819\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Automation_TestResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="10_ncr:8100000_{27004D7F-0B88-4528-8820-D5AB6785ED20}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32"/>
   <bookViews>
-    <workbookView windowHeight="6555" windowWidth="15990" xWindow="225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="1125"/>
+    <workbookView windowHeight="6555" windowWidth="15990" xWindow="225" yWindow="1125"/>
   </bookViews>
   <sheets>
     <sheet name="AEO 1971 - civil debt" r:id="rId1" sheetId="2"/>
@@ -887,7 +886,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
@@ -2769,14 +2768,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3005,7 +3004,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -3146,7 +3145,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -3316,7 +3315,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -3710,7 +3709,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -4038,7 +4037,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -4367,7 +4366,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -4768,7 +4767,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -5162,7 +5161,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -5429,7 +5428,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -8176,7 +8175,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -8582,7 +8581,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -8692,7 +8691,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -11282,7 +11281,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -11613,7 +11612,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -12022,7 +12021,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -12432,7 +12431,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -14772,7 +14771,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -15110,7 +15109,7 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -15517,7 +15516,7 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -15871,7 +15870,7 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -20571,7 +20570,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -20746,7 +20745,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -20948,7 +20947,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -21123,7 +21122,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -21296,7 +21295,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -21521,7 +21520,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C42365B-8A05-41D3-9A48-B444529A9B44}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -21536,7 +21535,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>

</xml_diff>

<commit_message>
completed the step3 of court order and student loan scneario one
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/TestOutPutResultFolder/201819 Payroll Court order and Student Loan Test result.xlsx
+++ b/Salesforce_Core_Framework/TestOutPutResultFolder/201819 Payroll Court order and Student Loan Test result.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Bajaj FinServe loan details\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Court Order and Student Loan Project\input sheet for scenario 1\Test Result output excel file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="8_{FB309530-861F-4D85-94BA-F06237EB3B39}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32"/>
+  <xr:revisionPtr documentId="10_ncr:8100000_{7D5AA2F0-CBD6-4650-B26B-59DFBE8BC93E}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32"/>
   <bookViews>
     <workbookView windowHeight="7545" windowWidth="20490" xWindow="0" xr2:uid="{7CD66A07-AC55-4110-B71A-2F0C233FAD1E}" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="This file is good" r:id="rId1" sheetId="1"/>
+    <sheet name="AEO1971civildebt" r:id="rId1" sheetId="1"/>
     <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="40">
   <si>
     <t>Scenario Name</t>
   </si>
@@ -115,13 +115,34 @@
     <t>TEST REMARKS</t>
   </si>
   <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payrun October-2018 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payrun November-2018 </t>
+  </si>
+  <si>
+    <t>30/11/2018</t>
+  </si>
+  <si>
+    <t>Court order: Effective to</t>
+  </si>
+  <si>
+    <t>GBP 50.00</t>
+  </si>
+  <si>
+    <t>GBP 950.00</t>
+  </si>
+  <si>
+    <t>GBP 713.24</t>
+  </si>
+  <si>
     <t>-</t>
   </si>
   <si>
     <t>GBP 0.00</t>
-  </si>
-  <si>
-    <t>TRUE</t>
   </si>
   <si>
     <t>FALSE</t>
@@ -250,7 +271,7 @@
       <color indexed="8"/>
     </font>
   </fonts>
-  <fills count="48">
+  <fills count="49">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,6 +335,12 @@
     <fill>
       <patternFill patternType="lightGray">
         <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
     <fill>
@@ -574,7 +601,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -585,92 +612,105 @@
     <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="7" fontId="1" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="8" fontId="2" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="3" fontId="4" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="7" fillId="8" fontId="4" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="7" fillId="8" fontId="2" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="4" fontId="1" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="5" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="2" fillId="0" fontId="6" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="3" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="7" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="9" fontId="1" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="10" fontId="1" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="3" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="6" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="7" fontId="1" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="8" fontId="2" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="3" fontId="4" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="7" fillId="8" fontId="4" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="7" fillId="8" fontId="2" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="4" fontId="1" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="5" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="2" fillId="0" fontId="6" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="3" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="7" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="9" fontId="1" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="10" fontId="1" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="7" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="11" fontId="8" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="4" fillId="4" fontId="4" numFmtId="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="4" fillId="5" fontId="4" numFmtId="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="5" fillId="5" fontId="4" numFmtId="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="13" fontId="9" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="14" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="16" fontId="10" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="17" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="19" fontId="11" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="20" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="22" fontId="12" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="23" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="25" fontId="13" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="26" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="28" fontId="14" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="29" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="31" fontId="15" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="32" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="34" fontId="16" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="35" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="37" fontId="17" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="38" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="40" fontId="18" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="41" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="43" fontId="19" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="44" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="46" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyFill="true"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="3" fontId="4" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="6" fillId="6" fontId="2" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="0" fontId="0" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="11" fontId="8" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="12" fontId="4" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="8" fontId="0" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="6" fontId="0" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="4" fillId="4" fontId="4" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="4" fillId="5" fontId="4" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="5" fillId="5" fontId="4" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="14" fontId="9" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="15" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="17" fontId="10" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="18" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="20" fontId="11" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="21" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="23" fontId="12" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="24" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="26" fontId="13" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="27" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="29" fontId="14" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="30" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="32" fontId="15" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="33" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="35" fontId="16" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="36" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="38" fontId="17" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="39" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="41" fontId="18" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="42" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="44" fontId="19" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="45" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="47" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="48" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -985,15 +1025,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B9A5757-7046-42A5-A0E8-107C80F83E5F}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="19.28515625" collapsed="true"/>
+  </cols>
   <sheetData>
-    <row ht="51.75" r="1" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="32.25" r="1" spans="1:15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1005,210 +1061,462 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
       <c r="J1" s="3"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="5"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="3"/>
       <c r="N1" s="3"/>
+      <c r="O1" s="18"/>
     </row>
-    <row ht="15.75" r="2" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="25" t="s">
+    <row ht="15.75" r="2" spans="1:15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="26" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="8" t="s">
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="9"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="18"/>
     </row>
-    <row ht="76.5" r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+    <row customHeight="1" ht="44.25" r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="6" t="s">
         <v>17</v>
       </c>
       <c r="N3" s="3"/>
+      <c r="O3" s="18"/>
     </row>
-    <row ht="60" r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+    <row customHeight="1" ht="35.25" r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="18" t="s">
+      <c r="I4" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="17" t="s">
+      <c r="K4" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="18" t="s">
+      <c r="L4" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="18" t="s">
+      <c r="M4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="20"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="18"/>
     </row>
-    <row ht="60" r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+    <row customHeight="1" ht="35.25" r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="N5" s="20"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="18"/>
     </row>
-    <row ht="45" r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+    <row customHeight="1" ht="30.75" r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" t="s" s="50">
+      <c r="B6" s="21"/>
+      <c r="C6" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="L6" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" s="3"/>
+      <c r="O6" s="18"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7">
+        <v>7</v>
+      </c>
+      <c r="I7">
+        <v>8</v>
+      </c>
+      <c r="J7">
+        <v>9</v>
+      </c>
+      <c r="K7">
+        <v>10</v>
+      </c>
+      <c r="L7">
+        <v>11</v>
+      </c>
+      <c r="M7">
+        <v>12</v>
+      </c>
+      <c r="N7">
+        <v>13</v>
+      </c>
+    </row>
+    <row ht="15.75" r="10" spans="1:15" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row ht="15.75" r="11" spans="1:15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="D6" t="s" s="50">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s" s="50">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s" s="50">
-        <v>31</v>
-      </c>
-      <c r="G6" t="s" s="50">
-        <v>31</v>
-      </c>
-      <c r="H6" t="s" s="50">
-        <v>31</v>
-      </c>
-      <c r="I6" t="s" s="50">
-        <v>31</v>
-      </c>
-      <c r="J6" t="s" s="50">
-        <v>31</v>
-      </c>
-      <c r="K6" t="s" s="50">
-        <v>31</v>
-      </c>
-      <c r="L6" t="s" s="50">
-        <v>31</v>
-      </c>
-      <c r="M6" t="s" s="50">
-        <v>31</v>
-      </c>
-      <c r="N6" s="20"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="M11" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="N11" s="25"/>
+      <c r="O11" s="18"/>
+    </row>
+    <row customHeight="1" ht="44.25" r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N12" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="O12" s="18"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="35.25" r="13" s="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="M13" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="35.25" r="14" s="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="11"/>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" t="s">
+        <v>34</v>
+      </c>
+      <c r="L14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M14" t="s">
+        <v>34</v>
+      </c>
+      <c r="N14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="30.75" r="15" s="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+      <c r="B15" s="21"/>
+      <c r="C15" t="s" s="51">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s" s="51">
+        <v>29</v>
+      </c>
+      <c r="E15" t="s" s="51">
+        <v>29</v>
+      </c>
+      <c r="F15" t="s" s="51">
+        <v>29</v>
+      </c>
+      <c r="G15" t="s" s="51">
+        <v>29</v>
+      </c>
+      <c r="H15" t="s" s="51">
+        <v>29</v>
+      </c>
+      <c r="I15" t="s" s="51">
+        <v>29</v>
+      </c>
+      <c r="J15" t="s" s="51">
+        <v>29</v>
+      </c>
+      <c r="K15" t="s" s="51">
+        <v>29</v>
+      </c>
+      <c r="L15" t="s" s="51">
+        <v>29</v>
+      </c>
+      <c r="M15" t="s" s="51">
+        <v>29</v>
+      </c>
+      <c r="N15" t="s" s="51">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="H2:K2"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="H11:K11"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
modifying the scenario 3
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/TestOutPutResultFolder/201819 Payroll Court order and Student Loan Test result.xlsx
+++ b/Salesforce_Core_Framework/TestOutPutResultFolder/201819 Payroll Court order and Student Loan Test result.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr documentId="10_ncr:8100800_{9E986543-FA84-4543-A6AE-F65E6F976473}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Court Order and Student Loan Project\input sheet for scenario 1\Test Result output excel file\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{16FE468D-50BD-411D-B72B-AB46936B652A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="4035" windowWidth="14160" xWindow="0" xr2:uid="{7CD66A07-AC55-4110-B71A-2F0C233FAD1E}" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="4035" activeTab="2" xr2:uid="{7CD66A07-AC55-4110-B71A-2F0C233FAD1E}"/>
   </bookViews>
   <sheets>
-    <sheet name="AEO1971civildebt" r:id="rId1" sheetId="1"/>
-    <sheet name="CAEO1971civildebt" r:id="rId2" sheetId="2"/>
+    <sheet name="AEO1971civildebt" sheetId="1" r:id="rId1"/>
+    <sheet name="CAEO1971civildebt" sheetId="2" r:id="rId2"/>
+    <sheet name="CAPS" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:G4"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="41">
   <si>
     <t>Scenario Name</t>
   </si>
@@ -138,24 +143,20 @@
     <t>CAEO 1971 - civil debt</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>GBP 0.00</t>
-  </si>
-  <si>
     <t>TRUE</t>
   </si>
   <si>
-    <t>FALSE</t>
+    <t>DO NOT TOUCH AUTOMATION EMP 110</t>
+  </si>
+  <si>
+    <t>CAPS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,127 +226,17 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
     </font>
   </fonts>
-  <fills count="86">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -423,315 +314,13 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
       <patternFill patternType="lightGray">
         <bgColor indexed="11"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
         <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
       </patternFill>
     </fill>
   </fills>
@@ -834,148 +423,105 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="2" fontId="2" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="7" fontId="1" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="8" fontId="2" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="3" fontId="4" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="7" fillId="8" fontId="4" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="7" fillId="8" fontId="2" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="4" fontId="1" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="5" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="2" fillId="0" fontId="6" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="3" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="7" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="9" fontId="1" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="10" fontId="1" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="3" fontId="4" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="6" fillId="6" fontId="2" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="0" fontId="0" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="11" fontId="4" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="8" fontId="0" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="6" fontId="0" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="12" fontId="8" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="13" fontId="9" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="4" fillId="4" fontId="4" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="4" fillId="5" fontId="4" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="5" fillId="5" fontId="4" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="15" fontId="11" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="16" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="18" fontId="12" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="19" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="21" fontId="13" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="22" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="24" fontId="14" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="25" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="27" fontId="15" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="28" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="30" fontId="16" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="31" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="33" fontId="17" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="34" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="36" fontId="18" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="37" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="39" fontId="19" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="40" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="42" fontId="20" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="43" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="45" fontId="21" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="46" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="48" fontId="22" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="49" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="51" fontId="23" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="52" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="54" fontId="24" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="55" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="57" fontId="25" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="58" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="60" fontId="26" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="61" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="63" fontId="27" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="64" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="66" fontId="28" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="67" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="69" fontId="29" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="70" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="72" fontId="30" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="73" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="75" fontId="31" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="76" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="78" fontId="32" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="79" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="81" fontId="33" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="82" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="34" fillId="84" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="85" borderId="0" xfId="0" applyFill="true"/>
+  <cellXfs count="34">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -992,10 +538,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1030,7 +576,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1082,7 +628,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1193,21 +739,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1224,7 +770,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1276,14 +822,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B9A5757-7046-42A5-A0E8-107C80F83E5F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B9A5757-7046-42A5-A0E8-107C80F83E5F}">
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1292,23 +838,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="34.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="1" max="1" width="23" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="19.28515625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="19.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="32.25" r="1" spans="1:15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1329,24 +875,24 @@
       <c r="N1" s="3"/>
       <c r="O1" s="18"/>
     </row>
-    <row ht="15.75" r="2" spans="1:15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="19"/>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="29" t="s">
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="30"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="32"/>
       <c r="L2" s="20" t="s">
         <v>4</v>
       </c>
@@ -1356,7 +902,7 @@
       <c r="N2" s="4"/>
       <c r="O2" s="18"/>
     </row>
-    <row customHeight="1" ht="44.25" r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -1399,7 +945,7 @@
       <c r="N3" s="3"/>
       <c r="O3" s="18"/>
     </row>
-    <row customHeight="1" ht="35.25" r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
@@ -1442,7 +988,7 @@
       <c r="N4" s="3"/>
       <c r="O4" s="18"/>
     </row>
-    <row customHeight="1" ht="35.25" r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>27</v>
       </c>
@@ -1452,7 +998,7 @@
       <c r="N5" s="3"/>
       <c r="O5" s="18"/>
     </row>
-    <row customHeight="1" ht="30.75" r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>28</v>
       </c>
@@ -1471,25 +1017,25 @@
       <c r="N6" s="3"/>
       <c r="O6" s="18"/>
     </row>
-    <row ht="15.75" r="10" spans="1:15" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row ht="15.75" r="11" spans="1:15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="19"/>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="29" t="s">
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="30"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="32"/>
       <c r="L11" s="20" t="s">
         <v>4</v>
       </c>
@@ -1499,7 +1045,7 @@
       <c r="N11" s="24"/>
       <c r="O11" s="18"/>
     </row>
-    <row customHeight="1" ht="44.25" r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
@@ -1544,7 +1090,7 @@
       </c>
       <c r="O12" s="18"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="35.25" r="13" s="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" s="18" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
@@ -1588,7 +1134,7 @@
         <v>31</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="35.25" r="14" s="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" s="18" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>19</v>
@@ -1606,7 +1152,7 @@
       <c r="M14"/>
       <c r="N14"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="30.75" r="15" s="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" s="18" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="21"/>
       <c r="C15" s="26"/>
@@ -1629,38 +1175,38 @@
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="H11:K11"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578A5A75-B72B-436E-8FAA-B21ABB37E878}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578A5A75-B72B-436E-8FAA-B21ABB37E878}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection sqref="A1:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="31.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="19.5703125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="51.75" r="1" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1680,24 +1226,24 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row ht="15.75" r="2" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="19"/>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="29" t="s">
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="30"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="32"/>
       <c r="L2" s="20" t="s">
         <v>4</v>
       </c>
@@ -1706,7 +1252,7 @@
       </c>
       <c r="N2" s="4"/>
     </row>
-    <row ht="76.5" r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -1748,7 +1294,7 @@
       </c>
       <c r="N3" s="3"/>
     </row>
-    <row ht="24" r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="24" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
@@ -1790,7 +1336,7 @@
       </c>
       <c r="N4" s="3"/>
     </row>
-    <row ht="24" r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="24" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>27</v>
       </c>
@@ -1832,65 +1378,65 @@
       </c>
       <c r="N5" s="3"/>
     </row>
-    <row ht="45" r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="21"/>
-      <c r="C6" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="J6" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="K6" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="L6" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="M6" s="53" t="s">
-        <v>40</v>
+      <c r="C6" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" s="28" t="s">
+        <v>38</v>
       </c>
       <c r="N6" s="3"/>
     </row>
-    <row ht="15.75" r="10" spans="1:14" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row ht="39" r="11" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:14" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="19"/>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="29" t="s">
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="30"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="32"/>
       <c r="L11" s="20" t="s">
         <v>4</v>
       </c>
@@ -1899,7 +1445,7 @@
       </c>
       <c r="N11" s="24"/>
     </row>
-    <row ht="76.5" r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
@@ -1943,7 +1489,7 @@
         <v>35</v>
       </c>
     </row>
-    <row ht="24" r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="24" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
@@ -1987,7 +1533,7 @@
         <v>31</v>
       </c>
     </row>
-    <row customHeight="1" ht="27.75" r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>36</v>
@@ -2032,41 +1578,41 @@
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="21"/>
-      <c r="C15" t="s" s="77">
-        <v>40</v>
-      </c>
-      <c r="D15" t="s" s="77">
-        <v>40</v>
-      </c>
-      <c r="E15" t="s" s="77">
-        <v>40</v>
-      </c>
-      <c r="F15" t="s" s="77">
-        <v>40</v>
-      </c>
-      <c r="G15" t="s" s="77">
-        <v>40</v>
-      </c>
-      <c r="H15" t="s" s="77">
-        <v>40</v>
-      </c>
-      <c r="I15" t="s" s="77">
-        <v>40</v>
-      </c>
-      <c r="J15" t="s" s="77">
-        <v>40</v>
-      </c>
-      <c r="K15" t="s" s="77">
-        <v>40</v>
-      </c>
-      <c r="L15" t="s" s="77">
-        <v>40</v>
-      </c>
-      <c r="M15" t="s" s="77">
-        <v>40</v>
-      </c>
-      <c r="N15" t="s" s="77">
-        <v>40</v>
+      <c r="C15" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="K15" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="L15" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="M15" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="N15" s="29" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2076,7 +1622,338 @@
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="H11:K11"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3971DBA-BDFC-49B4-B5B2-F5F9F002AAA9}">
+  <dimension ref="A1:N15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="4"/>
+    </row>
+    <row r="3" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:14" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="19"/>
+      <c r="C11" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="M11" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="N11" s="24"/>
+    </row>
+    <row r="12" spans="1:14" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N12" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="M13" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="H11:K11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
completed 3d court order scenario
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/TestOutPutResultFolder/201819 Payroll Court order and Student Loan Test result.xlsx
+++ b/Salesforce_Core_Framework/TestOutPutResultFolder/201819 Payroll Court order and Student Loan Test result.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Court Order and Student Loan Project\input sheet for scenario 1\Test Result output excel file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{16FE468D-50BD-411D-B72B-AB46936B652A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="10_ncr:8100000_{16FE468D-50BD-411D-B72B-AB46936B652A}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="4035" activeTab="2" xr2:uid="{7CD66A07-AC55-4110-B71A-2F0C233FAD1E}"/>
+    <workbookView activeTab="2" windowHeight="4035" windowWidth="14160" xWindow="0" xr2:uid="{7CD66A07-AC55-4110-B71A-2F0C233FAD1E}" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="AEO1971civildebt" sheetId="1" r:id="rId1"/>
-    <sheet name="CAEO1971civildebt" sheetId="2" r:id="rId2"/>
-    <sheet name="CAPS" sheetId="3" r:id="rId3"/>
+    <sheet name="AEO1971civildebt" r:id="rId1" sheetId="1"/>
+    <sheet name="CAEO1971civildebt" r:id="rId2" sheetId="2"/>
+    <sheet name="CAPS" r:id="rId3" sheetId="3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="44">
   <si>
     <t>Scenario Name</t>
   </si>
@@ -150,13 +150,23 @@
   </si>
   <si>
     <t>CAPS</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>GBP 0.00</t>
+  </si>
+  <si>
+    <t>FALSE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,8 +245,128 @@
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="88">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -321,6 +451,318 @@
     <fill>
       <patternFill patternType="lightGray">
         <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
       </patternFill>
     </fill>
   </fills>
@@ -423,105 +865,153 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+  <cellXfs count="82">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="2" fontId="2" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="7" fontId="1" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="8" fontId="2" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="3" fontId="4" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="7" fillId="8" fontId="4" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="7" fillId="8" fontId="2" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="4" fontId="1" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="5" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="2" fillId="0" fontId="6" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="3" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="7" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="9" fontId="1" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="10" fontId="1" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="3" fontId="4" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="6" fillId="6" fontId="2" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="0" fontId="0" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="11" fontId="4" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="8" fontId="0" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="6" fontId="0" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="12" fontId="8" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="13" fontId="9" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="14" fontId="11" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="15" fontId="12" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="4" fillId="4" fontId="4" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="4" fillId="5" fontId="4" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="5" fillId="5" fontId="4" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="10" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="17" fontId="13" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="18" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="20" fontId="14" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="21" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="23" fontId="15" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="24" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="26" fontId="16" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="27" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="29" fontId="17" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="30" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="32" fontId="18" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="33" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="35" fontId="19" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="36" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="38" fontId="20" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="39" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="41" fontId="21" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="42" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="44" fontId="22" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="45" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="47" fontId="23" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="48" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="50" fontId="24" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="51" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="53" fontId="25" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="54" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="56" fontId="26" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="57" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="59" fontId="27" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="60" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="62" fontId="28" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="63" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="65" fontId="29" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="66" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="68" fontId="30" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="69" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="71" fontId="31" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="72" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="74" fontId="32" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="75" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="77" fontId="33" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="78" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="80" fontId="34" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="81" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="83" fontId="35" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="84" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="36" fillId="86" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="87" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -538,10 +1028,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -576,7 +1066,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -628,7 +1118,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -739,21 +1229,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -770,7 +1260,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -822,14 +1312,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B9A5757-7046-42A5-A0E8-107C80F83E5F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B9A5757-7046-42A5-A0E8-107C80F83E5F}">
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -838,23 +1328,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="19.28515625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="19.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="19.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="32.25" r="1" spans="1:15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -875,7 +1365,7 @@
       <c r="N1" s="3"/>
       <c r="O1" s="18"/>
     </row>
-    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="2" spans="1:15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>29</v>
       </c>
@@ -902,7 +1392,7 @@
       <c r="N2" s="4"/>
       <c r="O2" s="18"/>
     </row>
-    <row r="3" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="44.25" r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -945,7 +1435,7 @@
       <c r="N3" s="3"/>
       <c r="O3" s="18"/>
     </row>
-    <row r="4" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="35.25" r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
@@ -988,7 +1478,7 @@
       <c r="N4" s="3"/>
       <c r="O4" s="18"/>
     </row>
-    <row r="5" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="35.25" r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>27</v>
       </c>
@@ -998,7 +1488,7 @@
       <c r="N5" s="3"/>
       <c r="O5" s="18"/>
     </row>
-    <row r="6" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30.75" r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>28</v>
       </c>
@@ -1017,8 +1507,8 @@
       <c r="N6" s="3"/>
       <c r="O6" s="18"/>
     </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="10" spans="1:15" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row ht="15.75" r="11" spans="1:15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>30</v>
       </c>
@@ -1045,7 +1535,7 @@
       <c r="N11" s="24"/>
       <c r="O11" s="18"/>
     </row>
-    <row r="12" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="44.25" r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
@@ -1090,7 +1580,7 @@
       </c>
       <c r="O12" s="18"/>
     </row>
-    <row r="13" spans="1:15" s="18" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="35.25" r="13" s="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
@@ -1134,7 +1624,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="18" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="35.25" r="14" s="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>19</v>
@@ -1152,7 +1642,7 @@
       <c r="M14"/>
       <c r="N14"/>
     </row>
-    <row r="15" spans="1:15" s="18" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="30.75" r="15" s="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="21"/>
       <c r="C15" s="26"/>
@@ -1175,13 +1665,13 @@
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="H11:K11"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578A5A75-B72B-436E-8FAA-B21ABB37E878}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578A5A75-B72B-436E-8FAA-B21ABB37E878}">
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
@@ -1190,23 +1680,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="21.42578125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="11.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="51.75" r="1" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1226,7 +1716,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="2" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>29</v>
       </c>
@@ -1252,7 +1742,7 @@
       </c>
       <c r="N2" s="4"/>
     </row>
-    <row r="3" spans="1:14" ht="76.5" x14ac:dyDescent="0.25">
+    <row ht="76.5" r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -1294,7 +1784,7 @@
       </c>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14" ht="24" x14ac:dyDescent="0.25">
+    <row ht="24" r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
@@ -1336,7 +1826,7 @@
       </c>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="1:14" ht="24" x14ac:dyDescent="0.25">
+    <row ht="24" r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>27</v>
       </c>
@@ -1378,7 +1868,7 @@
       </c>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>28</v>
       </c>
@@ -1418,8 +1908,8 @@
       </c>
       <c r="N6" s="3"/>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:14" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="10" spans="1:14" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row ht="39" r="11" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>30</v>
       </c>
@@ -1445,7 +1935,7 @@
       </c>
       <c r="N11" s="24"/>
     </row>
-    <row r="12" spans="1:14" ht="76.5" x14ac:dyDescent="0.25">
+    <row ht="76.5" r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
@@ -1489,7 +1979,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="24" x14ac:dyDescent="0.25">
+    <row ht="24" r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
@@ -1533,7 +2023,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="27.75" r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>36</v>
@@ -1622,13 +2112,13 @@
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="H11:K11"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3971DBA-BDFC-49B4-B5B2-F5F9F002AAA9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3971DBA-BDFC-49B4-B5B2-F5F9F002AAA9}">
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
@@ -1637,22 +2127,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
-    <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="11" max="11" width="20.42578125" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="28.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="51.75" r="1" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1672,7 +2162,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:14" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="26.25" r="2" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>29</v>
       </c>
@@ -1698,7 +2188,7 @@
       </c>
       <c r="N2" s="4"/>
     </row>
-    <row r="3" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="50.25" r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -1740,7 +2230,7 @@
       </c>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="36" r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
@@ -1782,35 +2272,90 @@
       </c>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="32.25" r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>39</v>
       </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" t="s">
+        <v>22</v>
+      </c>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="31.5" r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="21"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
+      <c r="C6" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" s="56" t="s">
+        <v>38</v>
+      </c>
       <c r="N6" s="3"/>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:14" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="10" spans="1:14" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row ht="39" r="11" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>30</v>
       </c>
@@ -1836,7 +2381,7 @@
       </c>
       <c r="N11" s="24"/>
     </row>
-    <row r="12" spans="1:14" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="43.5" r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
@@ -1880,7 +2425,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30.75" r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
@@ -1924,27 +2469,87 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="27.75" r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>39</v>
       </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" t="s">
+        <v>32</v>
+      </c>
+      <c r="L14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M14" t="s">
+        <v>32</v>
+      </c>
+      <c r="N14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="21"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="29"/>
+      <c r="C15" t="s" s="80">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s" s="80">
+        <v>38</v>
+      </c>
+      <c r="E15" t="s" s="80">
+        <v>38</v>
+      </c>
+      <c r="F15" t="s" s="80">
+        <v>38</v>
+      </c>
+      <c r="G15" t="s" s="80">
+        <v>38</v>
+      </c>
+      <c r="H15" t="s" s="80">
+        <v>38</v>
+      </c>
+      <c r="I15" t="s" s="80">
+        <v>38</v>
+      </c>
+      <c r="J15" t="s" s="80">
+        <v>38</v>
+      </c>
+      <c r="K15" t="s" s="80">
+        <v>38</v>
+      </c>
+      <c r="L15" t="s" s="80">
+        <v>38</v>
+      </c>
+      <c r="M15" t="s" s="80">
+        <v>38</v>
+      </c>
+      <c r="N15" t="s" s="80">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1953,7 +2558,7 @@
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="H11:K11"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modifying the scripts for 4th scenario
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/TestOutPutResultFolder/201819 Payroll Court order and Student Loan Test result.xlsx
+++ b/Salesforce_Core_Framework/TestOutPutResultFolder/201819 Payroll Court order and Student Loan Test result.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Court Order and Student Loan Project\input sheet for scenario 1\Test Result output excel file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="10_ncr:8100000_{16FE468D-50BD-411D-B72B-AB46936B652A}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8F4A13B1-3EA5-44D7-9D5E-D1D42B4B095D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="2" windowHeight="4035" windowWidth="14160" xWindow="0" xr2:uid="{7CD66A07-AC55-4110-B71A-2F0C233FAD1E}" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="4035" activeTab="2" xr2:uid="{7CD66A07-AC55-4110-B71A-2F0C233FAD1E}"/>
   </bookViews>
   <sheets>
-    <sheet name="AEO1971civildebt" r:id="rId1" sheetId="1"/>
-    <sheet name="CAEO1971civildebt" r:id="rId2" sheetId="2"/>
-    <sheet name="CAPS" r:id="rId3" sheetId="3"/>
+    <sheet name="AEO1971civildebt" sheetId="1" r:id="rId1"/>
+    <sheet name="CAEO1971civildebt" sheetId="2" r:id="rId2"/>
+    <sheet name="CAPS" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="41">
   <si>
     <t>Scenario Name</t>
   </si>
@@ -150,23 +150,13 @@
   </si>
   <si>
     <t>CAPS</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>GBP 0.00</t>
-  </si>
-  <si>
-    <t>FALSE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="37" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,16 +209,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF222222"/>
@@ -246,127 +226,17 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
     </font>
   </fonts>
-  <fills count="88">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -451,318 +321,6 @@
     <fill>
       <patternFill patternType="lightGray">
         <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
       </patternFill>
     </fill>
   </fills>
@@ -865,153 +423,105 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="2" fontId="2" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="7" fontId="1" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="8" fontId="2" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="3" fontId="4" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="7" fillId="8" fontId="4" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="7" fillId="8" fontId="2" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="4" fontId="1" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="5" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="2" fillId="0" fontId="6" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="3" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="7" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="9" fontId="1" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="10" fontId="1" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="3" fontId="4" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="6" fillId="6" fontId="2" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="0" fontId="0" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="11" fontId="4" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="8" fontId="0" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="6" fontId="0" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="12" fontId="8" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="13" fontId="9" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="14" fontId="11" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="15" fontId="12" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="4" fillId="4" fontId="4" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="4" fillId="5" fontId="4" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="5" fillId="5" fontId="4" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="10" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="17" fontId="13" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="18" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="20" fontId="14" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="21" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="23" fontId="15" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="24" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="26" fontId="16" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="27" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="29" fontId="17" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="30" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="32" fontId="18" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="33" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="35" fontId="19" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="36" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="38" fontId="20" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="39" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="41" fontId="21" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="42" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="44" fontId="22" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="45" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="47" fontId="23" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="48" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="50" fontId="24" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="51" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="53" fontId="25" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="54" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="56" fontId="26" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="57" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="59" fontId="27" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="60" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="62" fontId="28" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="63" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="65" fontId="29" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="66" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="68" fontId="30" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="69" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="71" fontId="31" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="72" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="74" fontId="32" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="75" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="77" fontId="33" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="78" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="80" fontId="34" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="81" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="83" fontId="35" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="84" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="36" fillId="86" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="87" borderId="0" xfId="0" applyFill="true"/>
+  <cellXfs count="34">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1028,10 +538,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1066,7 +576,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1118,7 +628,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1229,21 +739,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1260,7 +770,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1312,39 +822,39 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B9A5757-7046-42A5-A0E8-107C80F83E5F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B9A5757-7046-42A5-A0E8-107C80F83E5F}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="E7" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="34.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="1" max="1" width="23" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="19.28515625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="19.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="32.25" r="1" spans="1:15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1365,7 +875,7 @@
       <c r="N1" s="3"/>
       <c r="O1" s="18"/>
     </row>
-    <row ht="15.75" r="2" spans="1:15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>29</v>
       </c>
@@ -1392,7 +902,7 @@
       <c r="N2" s="4"/>
       <c r="O2" s="18"/>
     </row>
-    <row customHeight="1" ht="44.25" r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -1435,7 +945,7 @@
       <c r="N3" s="3"/>
       <c r="O3" s="18"/>
     </row>
-    <row customHeight="1" ht="35.25" r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
@@ -1478,37 +988,92 @@
       <c r="N4" s="3"/>
       <c r="O4" s="18"/>
     </row>
-    <row customHeight="1" ht="35.25" r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>19</v>
       </c>
+      <c r="C5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>22</v>
+      </c>
       <c r="N5" s="3"/>
       <c r="O5" s="18"/>
     </row>
-    <row customHeight="1" ht="30.75" r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="21"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
+      <c r="C6" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" s="26" t="s">
+        <v>38</v>
+      </c>
       <c r="N6" s="3"/>
       <c r="O6" s="18"/>
     </row>
-    <row ht="15.75" r="10" spans="1:15" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row ht="15.75" r="11" spans="1:15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>30</v>
       </c>
@@ -1532,10 +1097,10 @@
       <c r="M11" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="N11" s="24"/>
+      <c r="N11" s="23"/>
       <c r="O11" s="18"/>
     </row>
-    <row customHeight="1" ht="44.25" r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
@@ -1575,12 +1140,12 @@
       <c r="M12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="N12" s="23" t="s">
+      <c r="N12" s="33" t="s">
         <v>35</v>
       </c>
       <c r="O12" s="18"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="35.25" r="13" s="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" s="18" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
@@ -1624,39 +1189,87 @@
         <v>31</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="35.25" r="14" s="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" s="18" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14"/>
-      <c r="G14"/>
-      <c r="H14"/>
-      <c r="I14"/>
-      <c r="J14"/>
-      <c r="K14"/>
-      <c r="L14"/>
-      <c r="M14"/>
-      <c r="N14"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="30.75" r="15" s="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C14" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="M14" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" s="18" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="21"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="26"/>
+      <c r="C15" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="K15" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="L15" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="M15" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="N15" s="26" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1665,42 +1278,42 @@
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="H11:K11"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578A5A75-B72B-436E-8FAA-B21ABB37E878}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578A5A75-B72B-436E-8FAA-B21ABB37E878}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection sqref="A1:XFD17"/>
+    <sheetView topLeftCell="C6" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="31.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="19.5703125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="51.75" r="1" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="24" t="s">
         <v>37</v>
       </c>
       <c r="C1" s="3"/>
@@ -1716,7 +1329,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row ht="15.75" r="2" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>29</v>
       </c>
@@ -1742,7 +1355,7 @@
       </c>
       <c r="N2" s="4"/>
     </row>
-    <row ht="76.5" r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -1784,7 +1397,7 @@
       </c>
       <c r="N3" s="3"/>
     </row>
-    <row ht="24" r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="24" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
@@ -1826,7 +1439,7 @@
       </c>
       <c r="N4" s="3"/>
     </row>
-    <row ht="24" r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="24" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>27</v>
       </c>
@@ -1868,48 +1481,48 @@
       </c>
       <c r="N5" s="3"/>
     </row>
-    <row ht="45" r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="21"/>
-      <c r="C6" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="K6" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="L6" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="M6" s="28" t="s">
+      <c r="C6" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" s="25" t="s">
         <v>38</v>
       </c>
       <c r="N6" s="3"/>
     </row>
-    <row ht="15.75" r="10" spans="1:14" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row ht="39" r="11" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:14" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>30</v>
       </c>
@@ -1933,9 +1546,9 @@
       <c r="M11" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="N11" s="24"/>
-    </row>
-    <row ht="76.5" r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N11" s="23"/>
+    </row>
+    <row r="12" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
@@ -1975,11 +1588,11 @@
       <c r="M12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="N12" s="23" t="s">
+      <c r="N12" s="33" t="s">
         <v>35</v>
       </c>
     </row>
-    <row ht="24" r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="24" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
@@ -2023,7 +1636,7 @@
         <v>31</v>
       </c>
     </row>
-    <row customHeight="1" ht="27.75" r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>36</v>
@@ -2068,40 +1681,40 @@
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="21"/>
-      <c r="C15" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="H15" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="I15" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="J15" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="K15" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="L15" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="M15" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="N15" s="29" t="s">
+      <c r="C15" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="K15" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="L15" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="M15" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="N15" s="26" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2112,41 +1725,42 @@
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="H11:K11"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3971DBA-BDFC-49B4-B5B2-F5F9F002AAA9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3971DBA-BDFC-49B4-B5B2-F5F9F002AAA9}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="28.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="1" max="1" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.28515625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20.42578125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="51.75" r="1" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="27" t="s">
         <v>40</v>
       </c>
       <c r="C1" s="3"/>
@@ -2162,7 +1776,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row ht="26.25" r="2" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>29</v>
       </c>
@@ -2188,7 +1802,7 @@
       </c>
       <c r="N2" s="4"/>
     </row>
-    <row customHeight="1" ht="50.25" r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -2230,7 +1844,7 @@
       </c>
       <c r="N3" s="3"/>
     </row>
-    <row customHeight="1" ht="36" r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
@@ -2272,7 +1886,7 @@
       </c>
       <c r="N4" s="3"/>
     </row>
-    <row customHeight="1" ht="32.25" r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>27</v>
       </c>
@@ -2314,48 +1928,48 @@
       </c>
       <c r="N5" s="3"/>
     </row>
-    <row customHeight="1" ht="31.5" r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="21"/>
-      <c r="C6" s="56" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="56" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="56" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="56" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="56" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="56" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="56" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" s="56" t="s">
-        <v>38</v>
-      </c>
-      <c r="K6" s="56" t="s">
-        <v>38</v>
-      </c>
-      <c r="L6" s="56" t="s">
-        <v>38</v>
-      </c>
-      <c r="M6" s="56" t="s">
+      <c r="C6" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" s="28" t="s">
         <v>38</v>
       </c>
       <c r="N6" s="3"/>
     </row>
-    <row ht="15.75" r="10" spans="1:14" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row ht="39" r="11" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:14" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>30</v>
       </c>
@@ -2379,9 +1993,9 @@
       <c r="M11" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="N11" s="24"/>
-    </row>
-    <row customHeight="1" ht="43.5" r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N11" s="23"/>
+    </row>
+    <row r="12" spans="1:14" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
@@ -2421,11 +2035,11 @@
       <c r="M12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="N12" s="23" t="s">
+      <c r="N12" s="33" t="s">
         <v>35</v>
       </c>
     </row>
-    <row customHeight="1" ht="30.75" r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
@@ -2469,7 +2083,7 @@
         <v>31</v>
       </c>
     </row>
-    <row customHeight="1" ht="27.75" r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>39</v>
@@ -2514,40 +2128,40 @@
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="21"/>
-      <c r="C15" t="s" s="80">
-        <v>38</v>
-      </c>
-      <c r="D15" t="s" s="80">
-        <v>38</v>
-      </c>
-      <c r="E15" t="s" s="80">
-        <v>38</v>
-      </c>
-      <c r="F15" t="s" s="80">
-        <v>38</v>
-      </c>
-      <c r="G15" t="s" s="80">
-        <v>38</v>
-      </c>
-      <c r="H15" t="s" s="80">
-        <v>38</v>
-      </c>
-      <c r="I15" t="s" s="80">
-        <v>38</v>
-      </c>
-      <c r="J15" t="s" s="80">
-        <v>38</v>
-      </c>
-      <c r="K15" t="s" s="80">
-        <v>38</v>
-      </c>
-      <c r="L15" t="s" s="80">
-        <v>38</v>
-      </c>
-      <c r="M15" t="s" s="80">
-        <v>38</v>
-      </c>
-      <c r="N15" t="s" s="80">
+      <c r="C15" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="K15" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="L15" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="M15" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="N15" s="29" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2558,7 +2172,7 @@
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="H11:K11"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modifying the 4th scenario
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/TestOutPutResultFolder/201819 Payroll Court order and Student Loan Test result.xlsx
+++ b/Salesforce_Core_Framework/TestOutPutResultFolder/201819 Payroll Court order and Student Loan Test result.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Court Order and Student Loan Project\input sheet for scenario 1\Test Result output excel file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8F4A13B1-3EA5-44D7-9D5E-D1D42B4B095D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EFD6A67B-683C-4BDB-86EC-8BB6E26B33B5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="4035" activeTab="2" xr2:uid="{7CD66A07-AC55-4110-B71A-2F0C233FAD1E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="4035" activeTab="3" xr2:uid="{7CD66A07-AC55-4110-B71A-2F0C233FAD1E}"/>
   </bookViews>
   <sheets>
     <sheet name="AEO1971civildebt" sheetId="1" r:id="rId1"/>
     <sheet name="CAEO1971civildebt" sheetId="2" r:id="rId2"/>
     <sheet name="CAPS" sheetId="3" r:id="rId3"/>
+    <sheet name="PAEO1971Maintenance" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="47">
   <si>
     <t>Scenario Name</t>
   </si>
@@ -150,6 +151,24 @@
   </si>
   <si>
     <t>CAPS</t>
+  </si>
+  <si>
+    <t>DO NOT TOUCH AUTOMATION EMP 111</t>
+  </si>
+  <si>
+    <t>Total cost to employer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payrun December-2018 </t>
+  </si>
+  <si>
+    <t>PAEO1971Maintenance</t>
+  </si>
+  <si>
+    <t>GBP 1040.12</t>
+  </si>
+  <si>
+    <t>GBP 1000.00</t>
   </si>
 </sst>
 </file>
@@ -236,7 +255,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,8 +342,14 @@
         <bgColor indexed="11"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -421,11 +446,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -507,13 +558,34 @@
     <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -832,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B9A5757-7046-42A5-A0E8-107C80F83E5F}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView topLeftCell="E7" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,19 +952,19 @@
         <v>29</v>
       </c>
       <c r="B2" s="19"/>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="31" t="s">
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="32"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="34"/>
       <c r="L2" s="20" t="s">
         <v>4</v>
       </c>
@@ -1031,7 +1103,7 @@
       <c r="N5" s="3"/>
       <c r="O5" s="18"/>
     </row>
-    <row r="6" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>28</v>
       </c>
@@ -1078,19 +1150,19 @@
         <v>30</v>
       </c>
       <c r="B11" s="19"/>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="31" t="s">
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="32"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="34"/>
       <c r="L11" s="20" t="s">
         <v>4</v>
       </c>
@@ -1140,7 +1212,7 @@
       <c r="M12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="N12" s="33" t="s">
+      <c r="N12" s="31" t="s">
         <v>35</v>
       </c>
       <c r="O12" s="18"/>
@@ -1231,7 +1303,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="18" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" s="18" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="21"/>
       <c r="C15" s="26" t="s">
@@ -1287,8 +1359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578A5A75-B72B-436E-8FAA-B21ABB37E878}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView topLeftCell="C6" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,19 +1406,19 @@
         <v>29</v>
       </c>
       <c r="B2" s="19"/>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="31" t="s">
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="32"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="34"/>
       <c r="L2" s="20" t="s">
         <v>4</v>
       </c>
@@ -1481,7 +1553,7 @@
       </c>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>28</v>
       </c>
@@ -1527,19 +1599,19 @@
         <v>30</v>
       </c>
       <c r="B11" s="19"/>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="31" t="s">
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="32"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="34"/>
       <c r="L11" s="20" t="s">
         <v>4</v>
       </c>
@@ -1588,7 +1660,7 @@
       <c r="M12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="N12" s="33" t="s">
+      <c r="N12" s="31" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1678,7 +1750,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="21"/>
       <c r="C15" s="26" t="s">
@@ -1734,8 +1806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3971DBA-BDFC-49B4-B5B2-F5F9F002AAA9}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1781,19 +1853,19 @@
         <v>29</v>
       </c>
       <c r="B2" s="19"/>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="31" t="s">
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="32"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="34"/>
       <c r="L2" s="20" t="s">
         <v>4</v>
       </c>
@@ -1974,19 +2046,19 @@
         <v>30</v>
       </c>
       <c r="B11" s="19"/>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="31" t="s">
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="32"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="34"/>
       <c r="L11" s="20" t="s">
         <v>4</v>
       </c>
@@ -2035,7 +2107,7 @@
       <c r="M12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="N12" s="33" t="s">
+      <c r="N12" s="31" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2175,4 +2247,392 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2127CBC-8F6E-4E11-8815-584B931D5927}">
+  <dimension ref="A1:K24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="51" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="37" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="22"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" s="35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="51" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" s="36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13" s="37" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+    </row>
+    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="22"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="K20" s="35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="51" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K21" s="36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="H22" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="I22" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="K22" s="37" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15"/>
+      <c r="B23" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="16"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="F20:I20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
working on Reports for scenario5
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/TestOutPutResultFolder/201819 Payroll Court order and Student Loan Test result.xlsx
+++ b/Salesforce_Core_Framework/TestOutPutResultFolder/201819 Payroll Court order and Student Loan Test result.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Court Order and Student Loan Project\input sheet for scenario 1\Test Result output excel file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="10_ncr:8100000_{E29D3CAD-0332-4239-8B90-AA3288313A72}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{76E441CE-DA56-4910-8068-DFF1290F1EF4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="3" windowHeight="4035" windowWidth="14160" xWindow="0" xr2:uid="{7CD66A07-AC55-4110-B71A-2F0C233FAD1E}" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="4035" activeTab="4" xr2:uid="{7CD66A07-AC55-4110-B71A-2F0C233FAD1E}"/>
   </bookViews>
   <sheets>
-    <sheet name="AEO1971civildebt" r:id="rId1" sheetId="1"/>
-    <sheet name="CAEO1971civildebt" r:id="rId2" sheetId="2"/>
-    <sheet name="CAPS" r:id="rId3" sheetId="3"/>
-    <sheet name="PAEO1971Maintenance" r:id="rId4" sheetId="4"/>
+    <sheet name="AEO1971civildebt" sheetId="1" r:id="rId1"/>
+    <sheet name="CAEO1971civildebt" sheetId="2" r:id="rId2"/>
+    <sheet name="CAPS" sheetId="3" r:id="rId3"/>
+    <sheet name="PAEO1971Maintenance" sheetId="4" r:id="rId4"/>
+    <sheet name="PAEO1971Fine" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="53">
   <si>
     <t>Scenario Name</t>
   </si>
@@ -171,21 +172,29 @@
     <t>GBP 1,000.00</t>
   </si>
   <si>
-    <t>-</t>
+    <t>DO NOT TOUCH AUTOMATION EMP 112</t>
+  </si>
+  <si>
+    <t>Payment Shortfall contribution</t>
+  </si>
+  <si>
+    <t>Protected earnings contribution</t>
+  </si>
+  <si>
+    <t>Benefit Shortfall carry forward</t>
+  </si>
+  <si>
+    <t>GBP 949.00</t>
   </si>
   <si>
     <t>GBP 0.00</t>
-  </si>
-  <si>
-    <t>FALSE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="52" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,188 +292,8 @@
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
   </fonts>
-  <fills count="130">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -564,490 +393,12 @@
     </fill>
     <fill>
       <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
         <bgColor indexed="11"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="lightGray">
         <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray">
-        <bgColor indexed="51"/>
       </patternFill>
     </fill>
   </fills>
@@ -1176,203 +527,135 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="2" fontId="2" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="7" fontId="1" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="8" fontId="2" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="3" fontId="4" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="7" fillId="8" fontId="4" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="7" fillId="8" fontId="2" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="4" fontId="1" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="5" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="2" fillId="0" fontId="6" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="3" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="7" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="9" fontId="1" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="10" fontId="1" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="3" fontId="4" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="6" fillId="6" fontId="2" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="0" fontId="0" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="11" fontId="4" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="6" fontId="0" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="12" fontId="9" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="13" fontId="10" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="8" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="14" fontId="11" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="15" fontId="12" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="4" fillId="4" fontId="4" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="8" fontId="1" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="8" fillId="6" fontId="2" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="9" fillId="8" fontId="2" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="6" fontId="3" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="6" fontId="7" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="2" fillId="6" fontId="6" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="16" fontId="8" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="17" fontId="13" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="18" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="19" fontId="14" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="20" fontId="15" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="21" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="4" fillId="4" fontId="4" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="4" fillId="5" fontId="4" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="5" fillId="5" fontId="4" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="23" fontId="16" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="24" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="26" fontId="17" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="27" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="29" fontId="18" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="30" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="32" fontId="19" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="33" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="35" fontId="20" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="36" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="38" fontId="21" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="39" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="41" fontId="22" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="42" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="44" fontId="23" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="45" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="47" fontId="24" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="48" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="50" fontId="25" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="51" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="53" fontId="26" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="54" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="56" fontId="27" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="57" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="59" fontId="28" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="60" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="62" fontId="29" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="63" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="65" fontId="30" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="66" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="68" fontId="31" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="69" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="71" fontId="32" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="72" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="74" fontId="33" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="75" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="77" fontId="34" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="78" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="80" fontId="35" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="81" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="83" fontId="36" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="84" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="86" fontId="37" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="87" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="89" fontId="38" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="90" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="92" fontId="39" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="93" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="95" fontId="40" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="96" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="98" fontId="41" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="99" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="101" fontId="42" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="102" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="104" fontId="43" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="105" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="107" fontId="44" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="108" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="110" fontId="45" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="111" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="113" fontId="46" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="114" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="116" fontId="47" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="117" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="119" fontId="48" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="120" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="122" fontId="49" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="123" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="125" fontId="50" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="126" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="51" fillId="128" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="129" borderId="0" xfId="0" applyFill="true"/>
+  <cellXfs count="46">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1389,10 +672,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1427,7 +710,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1479,7 +762,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1590,21 +873,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1621,7 +904,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1673,14 +956,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B9A5757-7046-42A5-A0E8-107C80F83E5F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B9A5757-7046-42A5-A0E8-107C80F83E5F}">
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1689,23 +972,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="34.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="1" max="1" width="23" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="19.28515625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="19.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="32.25" r="1" spans="1:15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1726,24 +1009,24 @@
       <c r="N1" s="3"/>
       <c r="O1" s="18"/>
     </row>
-    <row ht="15.75" r="2" spans="1:15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="19"/>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="44" t="s">
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="45"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="44"/>
       <c r="L2" s="20" t="s">
         <v>4</v>
       </c>
@@ -1753,7 +1036,7 @@
       <c r="N2" s="4"/>
       <c r="O2" s="18"/>
     </row>
-    <row customHeight="1" ht="44.25" r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -1796,7 +1079,7 @@
       <c r="N3" s="3"/>
       <c r="O3" s="18"/>
     </row>
-    <row customHeight="1" ht="35.25" r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
@@ -1839,7 +1122,7 @@
       <c r="N4" s="3"/>
       <c r="O4" s="18"/>
     </row>
-    <row customHeight="1" ht="35.25" r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>27</v>
       </c>
@@ -1882,7 +1165,7 @@
       <c r="N5" s="3"/>
       <c r="O5" s="18"/>
     </row>
-    <row customHeight="1" ht="23.25" r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>28</v>
       </c>
@@ -1923,25 +1206,25 @@
       <c r="N6" s="3"/>
       <c r="O6" s="18"/>
     </row>
-    <row ht="15.75" r="10" spans="1:15" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row ht="15.75" r="11" spans="1:15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="19"/>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="44" t="s">
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="45"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="44"/>
       <c r="L11" s="20" t="s">
         <v>4</v>
       </c>
@@ -1951,7 +1234,7 @@
       <c r="N11" s="23"/>
       <c r="O11" s="18"/>
     </row>
-    <row customHeight="1" ht="44.25" r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
@@ -1996,7 +1279,7 @@
       </c>
       <c r="O12" s="18"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="35.25" r="13" s="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" s="18" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
@@ -2040,7 +1323,7 @@
         <v>31</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="35.25" r="14" s="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" s="18" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>19</v>
@@ -2082,7 +1365,7 @@
         <v>31</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="21.75" r="15" s="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" s="18" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="21"/>
       <c r="C15" s="26" t="s">
@@ -2129,13 +1412,13 @@
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="H11:K11"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578A5A75-B72B-436E-8FAA-B21ABB37E878}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578A5A75-B72B-436E-8FAA-B21ABB37E878}">
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -2144,23 +1427,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="31.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="19.5703125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="51.75" r="1" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2180,24 +1463,24 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row ht="15.75" r="2" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="19"/>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="44" t="s">
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="45"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="44"/>
       <c r="L2" s="20" t="s">
         <v>4</v>
       </c>
@@ -2206,7 +1489,7 @@
       </c>
       <c r="N2" s="4"/>
     </row>
-    <row ht="76.5" r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -2248,7 +1531,7 @@
       </c>
       <c r="N3" s="3"/>
     </row>
-    <row ht="24" r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="24" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
@@ -2290,7 +1573,7 @@
       </c>
       <c r="N4" s="3"/>
     </row>
-    <row ht="24" r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="24" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>27</v>
       </c>
@@ -2332,7 +1615,7 @@
       </c>
       <c r="N5" s="3"/>
     </row>
-    <row customHeight="1" ht="27.75" r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>28</v>
       </c>
@@ -2372,25 +1655,25 @@
       </c>
       <c r="N6" s="3"/>
     </row>
-    <row ht="15.75" r="10" spans="1:14" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row ht="15.75" r="11" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="19"/>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="44" t="s">
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="45"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="44"/>
       <c r="L11" s="20" t="s">
         <v>4</v>
       </c>
@@ -2399,7 +1682,7 @@
       </c>
       <c r="N11" s="23"/>
     </row>
-    <row ht="38.25" r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
@@ -2443,7 +1726,7 @@
         <v>35</v>
       </c>
     </row>
-    <row ht="24" r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="24" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
@@ -2487,7 +1770,7 @@
         <v>31</v>
       </c>
     </row>
-    <row customHeight="1" ht="27.75" r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>36</v>
@@ -2529,7 +1812,7 @@
         <v>31</v>
       </c>
     </row>
-    <row customHeight="1" ht="24.75" r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="21"/>
       <c r="C15" s="26" t="s">
@@ -2576,13 +1859,13 @@
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="H11:K11"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3971DBA-BDFC-49B4-B5B2-F5F9F002AAA9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3971DBA-BDFC-49B4-B5B2-F5F9F002AAA9}">
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -2591,23 +1874,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="28.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="1" max="1" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.28515625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20.42578125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="51.75" r="1" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2627,24 +1910,24 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row ht="26.25" r="2" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="19"/>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="44" t="s">
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="45"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="44"/>
       <c r="L2" s="20" t="s">
         <v>4</v>
       </c>
@@ -2653,7 +1936,7 @@
       </c>
       <c r="N2" s="4"/>
     </row>
-    <row customHeight="1" ht="50.25" r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -2695,7 +1978,7 @@
       </c>
       <c r="N3" s="3"/>
     </row>
-    <row customHeight="1" ht="36" r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
@@ -2737,7 +2020,7 @@
       </c>
       <c r="N4" s="3"/>
     </row>
-    <row customHeight="1" ht="32.25" r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>27</v>
       </c>
@@ -2779,7 +2062,7 @@
       </c>
       <c r="N5" s="3"/>
     </row>
-    <row customHeight="1" ht="31.5" r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>28</v>
       </c>
@@ -2819,25 +2102,25 @@
       </c>
       <c r="N6" s="3"/>
     </row>
-    <row ht="15.75" r="10" spans="1:14" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row ht="26.25" r="11" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:14" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="19"/>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="44" t="s">
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="45"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="44"/>
       <c r="L11" s="20" t="s">
         <v>4</v>
       </c>
@@ -2846,7 +2129,7 @@
       </c>
       <c r="N11" s="23"/>
     </row>
-    <row customHeight="1" ht="43.5" r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
@@ -2890,7 +2173,7 @@
         <v>35</v>
       </c>
     </row>
-    <row customHeight="1" ht="30.75" r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
@@ -2934,7 +2217,7 @@
         <v>31</v>
       </c>
     </row>
-    <row customHeight="1" ht="27.75" r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>39</v>
@@ -3023,35 +2306,35 @@
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="H11:K11"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2127CBC-8F6E-4E11-8815-584B931D5927}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2127CBC-8F6E-4E11-8815-584B931D5927}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection sqref="A1:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="35.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="1" max="1" width="22.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="15.75" r="1" spans="1:11" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3067,7 +2350,7 @@
       <c r="J1" s="17"/>
       <c r="K1" s="3"/>
     </row>
-    <row customHeight="1" ht="39" r="2" spans="1:11" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>29</v>
       </c>
@@ -3075,12 +2358,12 @@
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
       <c r="E2" s="30"/>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="45"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="44"/>
       <c r="J2" s="20" t="s">
         <v>4</v>
       </c>
@@ -3088,7 +2371,7 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="51" r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="51" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -3123,7 +2406,7 @@
         <v>17</v>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
@@ -3158,7 +2441,7 @@
         <v>22</v>
       </c>
     </row>
-    <row customHeight="1" ht="27.75" r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>27</v>
       </c>
@@ -3193,54 +2476,54 @@
         <v>22</v>
       </c>
     </row>
-    <row customHeight="1" ht="27" r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="21"/>
-      <c r="C6" s="68" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="68" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="68" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="68" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="68" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="68" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="68" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" s="68" t="s">
-        <v>38</v>
-      </c>
-      <c r="K6" s="68" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row ht="15.75" r="10" spans="1:11" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row ht="26.25" r="11" spans="1:11" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="22"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="44" t="s">
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="45"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="44"/>
       <c r="J11" s="20" t="s">
         <v>4</v>
       </c>
@@ -3248,7 +2531,7 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="51" r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="51" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
@@ -3283,7 +2566,7 @@
         <v>17</v>
       </c>
     </row>
-    <row customHeight="1" ht="34.5" r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
@@ -3318,7 +2601,7 @@
         <v>22</v>
       </c>
     </row>
-    <row customHeight="1" ht="33.75" r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>41</v>
@@ -3351,52 +2634,52 @@
         <v>22</v>
       </c>
     </row>
-    <row customHeight="1" ht="21.75" r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="21"/>
-      <c r="C15" t="s" s="116">
-        <v>38</v>
-      </c>
-      <c r="D15" t="s" s="116">
-        <v>38</v>
-      </c>
-      <c r="E15" t="s" s="116">
-        <v>38</v>
-      </c>
-      <c r="F15" t="s" s="116">
-        <v>38</v>
-      </c>
-      <c r="G15" t="s" s="116">
-        <v>38</v>
-      </c>
-      <c r="H15" t="s" s="116">
-        <v>38</v>
-      </c>
-      <c r="I15" t="s" s="116">
-        <v>38</v>
-      </c>
-      <c r="J15" t="s" s="116">
-        <v>38</v>
-      </c>
-      <c r="K15" t="s" s="116">
-        <v>38</v>
-      </c>
-    </row>
-    <row ht="15.75" r="19" spans="1:11" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row ht="26.25" r="20" spans="1:11" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="K15" s="41" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="22" t="s">
         <v>43</v>
       </c>
       <c r="B20" s="22"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="44" t="s">
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="45"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="44"/>
       <c r="J20" s="20" t="s">
         <v>4</v>
       </c>
@@ -3404,7 +2687,7 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="51" r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="51" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>6</v>
       </c>
@@ -3439,7 +2722,7 @@
         <v>17</v>
       </c>
     </row>
-    <row customHeight="1" ht="34.5" r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>18</v>
       </c>
@@ -3474,7 +2757,7 @@
         <v>22</v>
       </c>
     </row>
-    <row customHeight="1" ht="33.75" r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
       <c r="B23" s="11" t="s">
         <v>41</v>
@@ -3507,34 +2790,34 @@
         <v>22</v>
       </c>
     </row>
-    <row customHeight="1" ht="25.5" r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16"/>
       <c r="B24" s="21"/>
-      <c r="C24" s="92" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="92" t="s">
-        <v>38</v>
-      </c>
-      <c r="E24" s="92" t="s">
-        <v>38</v>
-      </c>
-      <c r="F24" s="92" t="s">
-        <v>38</v>
-      </c>
-      <c r="G24" s="92" t="s">
-        <v>38</v>
-      </c>
-      <c r="H24" s="92" t="s">
-        <v>38</v>
-      </c>
-      <c r="I24" s="92" t="s">
-        <v>38</v>
-      </c>
-      <c r="J24" s="92" t="s">
-        <v>38</v>
-      </c>
-      <c r="K24" s="92" t="s">
+      <c r="C24" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="G24" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="H24" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="I24" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="J24" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="K24" s="40" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3546,7 +2829,473 @@
     <mergeCell ref="C20:E20"/>
     <mergeCell ref="F20:I20"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18DF2305-D886-4933-9EB5-D5C6CA8728D8}">
+  <dimension ref="A1:N24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.7109375" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="26" customWidth="1"/>
+    <col min="10" max="10" width="25.5703125" customWidth="1"/>
+    <col min="11" max="11" width="29.140625" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" customWidth="1"/>
+    <col min="13" max="13" width="18.5703125" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="K4" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+    </row>
+    <row r="6" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="45"/>
+      <c r="L6" s="45"/>
+      <c r="M6" s="45"/>
+      <c r="N6" s="45"/>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="22"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="N11" s="32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N12" s="33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="M13" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="N13" s="34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="41"/>
+      <c r="L15" s="41"/>
+      <c r="M15" s="41"/>
+      <c r="N15" s="41"/>
+    </row>
+    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="22"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="43"/>
+      <c r="L20" s="44"/>
+      <c r="M20" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="N20" s="32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N21" s="33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="H22" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="M22" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="N22" s="34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15"/>
+      <c r="B23" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="16"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="40"/>
+      <c r="M24" s="40"/>
+      <c r="N24" s="40"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="F2:L2"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="F11:L11"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="F20:L20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
nov report worked out
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/TestOutPutResultFolder/201819 Payroll Court order and Student Loan Test result.xlsx
+++ b/Salesforce_Core_Framework/TestOutPutResultFolder/201819 Payroll Court order and Student Loan Test result.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Court Order and Student Loan Project\input sheet for scenario 1\Test Result output excel file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{76E441CE-DA56-4910-8068-DFF1290F1EF4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="10_ncr:8100000_{6D5A3130-E06A-4260-9629-B6A9569D4622}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="4035" activeTab="4" xr2:uid="{7CD66A07-AC55-4110-B71A-2F0C233FAD1E}"/>
+    <workbookView activeTab="4" windowHeight="4035" windowWidth="14160" xWindow="0" xr2:uid="{7CD66A07-AC55-4110-B71A-2F0C233FAD1E}" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="AEO1971civildebt" sheetId="1" r:id="rId1"/>
-    <sheet name="CAEO1971civildebt" sheetId="2" r:id="rId2"/>
-    <sheet name="CAPS" sheetId="3" r:id="rId3"/>
-    <sheet name="PAEO1971Maintenance" sheetId="4" r:id="rId4"/>
-    <sheet name="PAEO1971Fine" sheetId="5" r:id="rId5"/>
+    <sheet name="AEO1971civildebt" r:id="rId1" sheetId="1"/>
+    <sheet name="CAEO1971civildebt" r:id="rId2" sheetId="2"/>
+    <sheet name="CAPS" r:id="rId3" sheetId="3"/>
+    <sheet name="PAEO1971Maintenance" r:id="rId4" sheetId="4"/>
+    <sheet name="PAEO1971Fine" r:id="rId5" sheetId="5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="65">
   <si>
     <t>Scenario Name</t>
   </si>
@@ -181,20 +181,57 @@
     <t>Protected earnings contribution</t>
   </si>
   <si>
-    <t>Benefit Shortfall carry forward</t>
-  </si>
-  <si>
     <t>GBP 949.00</t>
   </si>
   <si>
     <t>GBP 0.00</t>
+  </si>
+  <si>
+    <t>Payrun January-2019</t>
+  </si>
+  <si>
+    <t>GBP 150.00</t>
+  </si>
+  <si>
+    <t>GBP 1,449.00</t>
+  </si>
+  <si>
+    <t>GBP 1,600.00</t>
+  </si>
+  <si>
+    <t>GBP -50.00</t>
+  </si>
+  <si>
+    <t>GBP 1,450.00</t>
+  </si>
+  <si>
+    <t>GBP 600.00</t>
+  </si>
+  <si>
+    <t>GBP 350.00</t>
+  </si>
+  <si>
+    <t>GBP 1,350.00</t>
+  </si>
+  <si>
+    <t>Protected earnings carried forward</t>
+  </si>
+  <si>
+    <t>Benefit Shortfall carry forward(court order shortfall carry forward)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>FALSE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="67" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,8 +329,263 @@
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
   </fonts>
-  <fills count="20">
+  <fills count="173">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -401,8 +693,671 @@
         <bgColor indexed="11"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -525,137 +1480,262 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="154">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="2" fontId="2" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="7" fontId="1" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="8" fontId="2" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="3" fontId="4" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="7" fillId="8" fontId="4" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="7" fillId="8" fontId="2" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="4" fontId="1" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="5" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="2" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="3" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="7" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="9" fontId="1" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="10" fontId="1" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="3" fontId="4" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="6" fillId="6" fontId="2" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="11" fontId="4" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="6" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="12" fontId="9" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="13" fontId="10" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="8" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="14" fontId="11" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="15" fontId="12" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="4" fillId="4" fontId="4" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="8" fontId="1" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="8" fillId="6" fontId="2" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="9" fillId="8" fontId="2" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="6" fontId="3" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="6" fontId="7" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="2" fillId="6" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="16" fontId="8" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="4" fillId="4" fontId="4" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="17" fontId="13" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="18" fontId="14" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="19" fontId="15" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="17" fontId="13" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="4" fillId="4" fontId="4" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="4" fillId="5" fontId="4" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="5" fillId="5" fontId="4" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="10" fillId="6" fontId="3" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyBorder="1" applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="21" fontId="16" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="22" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="24" fontId="17" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="25" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="27" fontId="18" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="28" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="30" fontId="19" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="31" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="33" fontId="20" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="34" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="36" fontId="21" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="37" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="39" fontId="22" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="40" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="42" fontId="23" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="43" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="45" fontId="24" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="46" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="48" fontId="25" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="49" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="51" fontId="26" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="52" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="54" fontId="27" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="55" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="57" fontId="28" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="58" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="60" fontId="29" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="61" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="63" fontId="30" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="64" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="66" fontId="31" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="67" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="69" fontId="32" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="70" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="72" fontId="33" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="73" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="75" fontId="34" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="76" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="78" fontId="35" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="79" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="81" fontId="36" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="82" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="84" fontId="37" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="85" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="87" fontId="38" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="88" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="90" fontId="39" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="91" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="93" fontId="40" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="94" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="96" fontId="41" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="97" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="99" fontId="42" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="100" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="102" fontId="43" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="103" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="105" fontId="44" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="106" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="108" fontId="45" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="109" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="111" fontId="46" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="112" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="114" fontId="47" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="115" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="117" fontId="48" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="118" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="120" fontId="49" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="121" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="123" fontId="50" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="124" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="126" fontId="51" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="127" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="129" fontId="52" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="130" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="132" fontId="53" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="133" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="135" fontId="54" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="136" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="138" fontId="55" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="139" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="141" fontId="56" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="142" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="144" fontId="57" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="145" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="147" fontId="58" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="148" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="150" fontId="59" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="151" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="153" fontId="60" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="154" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="156" fontId="61" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="157" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="159" fontId="62" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="160" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="162" fontId="63" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="163" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="165" fontId="64" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="166" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="168" fontId="65" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="169" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="66" fillId="171" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="172" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -672,10 +1752,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -710,7 +1790,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -762,7 +1842,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -873,21 +1953,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -904,7 +1984,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -956,14 +2036,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B9A5757-7046-42A5-A0E8-107C80F83E5F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B9A5757-7046-42A5-A0E8-107C80F83E5F}">
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -972,23 +2052,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="19.28515625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="19.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="19.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="32.25" r="1" spans="1:15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1009,24 +2089,24 @@
       <c r="N1" s="3"/>
       <c r="O1" s="18"/>
     </row>
-    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="2" spans="1:15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="19"/>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="43" t="s">
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="45"/>
       <c r="L2" s="20" t="s">
         <v>4</v>
       </c>
@@ -1036,7 +2116,7 @@
       <c r="N2" s="4"/>
       <c r="O2" s="18"/>
     </row>
-    <row r="3" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="44.25" r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -1079,7 +2159,7 @@
       <c r="N3" s="3"/>
       <c r="O3" s="18"/>
     </row>
-    <row r="4" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="35.25" r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
@@ -1122,7 +2202,7 @@
       <c r="N4" s="3"/>
       <c r="O4" s="18"/>
     </row>
-    <row r="5" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="35.25" r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>27</v>
       </c>
@@ -1165,7 +2245,7 @@
       <c r="N5" s="3"/>
       <c r="O5" s="18"/>
     </row>
-    <row r="6" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="23.25" r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>28</v>
       </c>
@@ -1206,25 +2286,25 @@
       <c r="N6" s="3"/>
       <c r="O6" s="18"/>
     </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="10" spans="1:15" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row ht="15.75" r="11" spans="1:15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="19"/>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="43" t="s">
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="45"/>
       <c r="L11" s="20" t="s">
         <v>4</v>
       </c>
@@ -1234,7 +2314,7 @@
       <c r="N11" s="23"/>
       <c r="O11" s="18"/>
     </row>
-    <row r="12" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="44.25" r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
@@ -1279,7 +2359,7 @@
       </c>
       <c r="O12" s="18"/>
     </row>
-    <row r="13" spans="1:15" s="18" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="35.25" r="13" s="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
@@ -1323,7 +2403,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="18" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="35.25" r="14" s="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>19</v>
@@ -1365,7 +2445,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="18" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="21.75" r="15" s="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="21"/>
       <c r="C15" s="26" t="s">
@@ -1412,13 +2492,13 @@
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="H11:K11"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578A5A75-B72B-436E-8FAA-B21ABB37E878}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578A5A75-B72B-436E-8FAA-B21ABB37E878}">
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -1427,23 +2507,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="21.42578125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="11.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="51.75" r="1" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1463,24 +2543,24 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="2" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="19"/>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="43" t="s">
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="45"/>
       <c r="L2" s="20" t="s">
         <v>4</v>
       </c>
@@ -1489,7 +2569,7 @@
       </c>
       <c r="N2" s="4"/>
     </row>
-    <row r="3" spans="1:14" ht="76.5" x14ac:dyDescent="0.25">
+    <row ht="76.5" r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -1531,7 +2611,7 @@
       </c>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14" ht="24" x14ac:dyDescent="0.25">
+    <row ht="24" r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
@@ -1573,7 +2653,7 @@
       </c>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="1:14" ht="24" x14ac:dyDescent="0.25">
+    <row ht="24" r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>27</v>
       </c>
@@ -1615,7 +2695,7 @@
       </c>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="27.75" r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>28</v>
       </c>
@@ -1655,25 +2735,25 @@
       </c>
       <c r="N6" s="3"/>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="10" spans="1:14" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row ht="15.75" r="11" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="19"/>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="43" t="s">
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="45"/>
       <c r="L11" s="20" t="s">
         <v>4</v>
       </c>
@@ -1682,7 +2762,7 @@
       </c>
       <c r="N11" s="23"/>
     </row>
-    <row r="12" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+    <row ht="38.25" r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
@@ -1726,7 +2806,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="24" x14ac:dyDescent="0.25">
+    <row ht="24" r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
@@ -1770,7 +2850,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="27.75" r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>36</v>
@@ -1812,7 +2892,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="24.75" r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="21"/>
       <c r="C15" s="26" t="s">
@@ -1859,13 +2939,13 @@
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="H11:K11"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3971DBA-BDFC-49B4-B5B2-F5F9F002AAA9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3971DBA-BDFC-49B4-B5B2-F5F9F002AAA9}">
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -1874,23 +2954,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.42578125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="28.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="13.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="51.75" r="1" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1910,24 +2990,24 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:14" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="26.25" r="2" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="19"/>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="43" t="s">
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="45"/>
       <c r="L2" s="20" t="s">
         <v>4</v>
       </c>
@@ -1936,7 +3016,7 @@
       </c>
       <c r="N2" s="4"/>
     </row>
-    <row r="3" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="50.25" r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -1978,7 +3058,7 @@
       </c>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="36" r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
@@ -2020,7 +3100,7 @@
       </c>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="32.25" r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>27</v>
       </c>
@@ -2062,7 +3142,7 @@
       </c>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="31.5" r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>28</v>
       </c>
@@ -2102,25 +3182,25 @@
       </c>
       <c r="N6" s="3"/>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:14" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="10" spans="1:14" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row ht="26.25" r="11" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="19"/>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="43" t="s">
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="45"/>
       <c r="L11" s="20" t="s">
         <v>4</v>
       </c>
@@ -2129,7 +3209,7 @@
       </c>
       <c r="N11" s="23"/>
     </row>
-    <row r="12" spans="1:14" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="43.5" r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
@@ -2173,7 +3253,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30.75" r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
@@ -2217,7 +3297,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="27.75" r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>39</v>
@@ -2306,13 +3386,13 @@
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="H11:K11"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2127CBC-8F6E-4E11-8815-584B931D5927}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2127CBC-8F6E-4E11-8815-584B931D5927}">
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
@@ -2321,20 +3401,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="1" spans="1:11" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2350,7 +3430,7 @@
       <c r="J1" s="17"/>
       <c r="K1" s="3"/>
     </row>
-    <row r="2" spans="1:11" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="39" r="2" spans="1:11" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>29</v>
       </c>
@@ -2358,12 +3438,12 @@
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
       <c r="E2" s="30"/>
-      <c r="F2" s="43" t="s">
+      <c r="F2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="45"/>
       <c r="J2" s="20" t="s">
         <v>4</v>
       </c>
@@ -2371,7 +3451,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="51" x14ac:dyDescent="0.25">
+    <row ht="51" r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -2406,7 +3486,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
@@ -2441,7 +3521,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="27.75" r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>27</v>
       </c>
@@ -2476,7 +3556,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="27" r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>28</v>
       </c>
@@ -2509,21 +3589,21 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="10" spans="1:11" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row ht="26.25" r="11" spans="1:11" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="22"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="43" t="s">
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="45"/>
       <c r="J11" s="20" t="s">
         <v>4</v>
       </c>
@@ -2531,7 +3611,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="51" x14ac:dyDescent="0.25">
+    <row ht="51" r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
@@ -2566,7 +3646,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="34.5" r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
@@ -2601,7 +3681,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="33.75" r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>41</v>
@@ -2634,7 +3714,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="21.75" r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="21"/>
       <c r="C15" s="41" t="s">
@@ -2665,21 +3745,21 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="19" spans="1:11" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row ht="26.25" r="20" spans="1:11" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="22" t="s">
         <v>43</v>
       </c>
       <c r="B20" s="22"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="43" t="s">
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="G20" s="43"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="45"/>
       <c r="J20" s="20" t="s">
         <v>4</v>
       </c>
@@ -2687,7 +3767,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="51" x14ac:dyDescent="0.25">
+    <row ht="51" r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>6</v>
       </c>
@@ -2722,7 +3802,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="34.5" r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>18</v>
       </c>
@@ -2757,7 +3837,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="33.75" r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
       <c r="B23" s="11" t="s">
         <v>41</v>
@@ -2790,7 +3870,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="25.5" r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="16"/>
       <c r="B24" s="21"/>
       <c r="C24" s="40" t="s">
@@ -2829,14 +3909,14 @@
     <mergeCell ref="C20:E20"/>
     <mergeCell ref="F20:I20"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18DF2305-D886-4933-9EB5-D5C6CA8728D8}">
-  <dimension ref="A1:N24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18DF2305-D886-4933-9EB5-D5C6CA8728D8}">
+  <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
@@ -2844,23 +3924,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
-    <col min="9" max="9" width="26" customWidth="1"/>
-    <col min="10" max="10" width="25.5703125" customWidth="1"/>
-    <col min="11" max="11" width="29.140625" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" customWidth="1"/>
-    <col min="13" max="13" width="18.5703125" customWidth="1"/>
-    <col min="14" max="14" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="28.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="17.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="1" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2879,7 +3959,7 @@
       <c r="M1" s="17"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="39" r="2" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>29</v>
       </c>
@@ -2887,15 +3967,15 @@
       <c r="C2" s="38"/>
       <c r="D2" s="38"/>
       <c r="E2" s="38"/>
-      <c r="F2" s="43" t="s">
+      <c r="F2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="45"/>
       <c r="M2" s="20" t="s">
         <v>4</v>
       </c>
@@ -2903,7 +3983,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+    <row ht="38.25" r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -2935,7 +4015,7 @@
         <v>49</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>15</v>
@@ -2947,7 +4027,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
@@ -2961,7 +4041,7 @@
         <v>33</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F4" s="36" t="s">
         <v>22</v>
@@ -2976,7 +4056,7 @@
         <v>32</v>
       </c>
       <c r="J4" s="36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K4" s="36" t="s">
         <v>32</v>
@@ -2991,62 +4071,110 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="27.75" r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-    </row>
-    <row r="6" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5" t="s">
+        <v>26</v>
+      </c>
+      <c r="N5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="27" r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="21"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
-    </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="122" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="122" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="122" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="122" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="122" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="122" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="122" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="122" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="123" t="s">
+        <v>64</v>
+      </c>
+      <c r="L6" s="122" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" s="122" t="s">
+        <v>38</v>
+      </c>
+      <c r="N6" s="122" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row ht="15.75" r="10" spans="1:14" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row ht="15.75" r="11" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="22"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="43" t="s">
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="43"/>
-      <c r="L11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="45"/>
       <c r="M11" s="20" t="s">
         <v>4</v>
       </c>
@@ -3054,7 +4182,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+    <row ht="38.25" r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
@@ -3086,7 +4214,7 @@
         <v>49</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="L12" s="6" t="s">
         <v>15</v>
@@ -3098,7 +4226,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="34.5" r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
@@ -3106,84 +4234,146 @@
         <v>47</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="F13" s="36" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H13" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
+        <v>33</v>
+      </c>
+      <c r="I13" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="J13" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="K13" s="34" t="s">
+        <v>51</v>
+      </c>
       <c r="L13" s="36" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="M13" s="34" t="s">
         <v>26</v>
       </c>
       <c r="N13" s="34" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="33.75" r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I14" t="s">
+        <v>56</v>
+      </c>
+      <c r="J14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" t="s">
+        <v>53</v>
+      </c>
+      <c r="M14" t="s">
+        <v>26</v>
+      </c>
+      <c r="N14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="21.75" r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="21"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="41"/>
-      <c r="L15" s="41"/>
-      <c r="M15" s="41"/>
-      <c r="N15" s="41"/>
-    </row>
-    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" t="s" s="152">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s" s="152">
+        <v>38</v>
+      </c>
+      <c r="E15" t="s" s="152">
+        <v>38</v>
+      </c>
+      <c r="F15" t="s" s="152">
+        <v>38</v>
+      </c>
+      <c r="G15" t="s" s="152">
+        <v>38</v>
+      </c>
+      <c r="H15" t="s" s="152">
+        <v>38</v>
+      </c>
+      <c r="I15" t="s" s="152">
+        <v>38</v>
+      </c>
+      <c r="J15" t="s" s="152">
+        <v>38</v>
+      </c>
+      <c r="K15" t="s" s="153">
+        <v>64</v>
+      </c>
+      <c r="L15" t="s" s="152">
+        <v>38</v>
+      </c>
+      <c r="M15" t="s" s="152">
+        <v>38</v>
+      </c>
+      <c r="N15" t="s" s="152">
+        <v>38</v>
+      </c>
+    </row>
+    <row ht="15.75" r="19" spans="1:14" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row ht="15.75" r="20" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="22" t="s">
         <v>43</v>
       </c>
       <c r="B20" s="22"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="43" t="s">
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="G20" s="43"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="43"/>
-      <c r="K20" s="43"/>
-      <c r="L20" s="44"/>
-      <c r="M20" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="N20" s="32" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
+      <c r="K20" s="44"/>
+      <c r="L20" s="45"/>
+      <c r="M20" s="32"/>
+      <c r="N20" s="48"/>
+    </row>
+    <row ht="38.25" r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>6</v>
       </c>
@@ -3215,19 +4405,17 @@
         <v>49</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="L21" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="M21" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="M21" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="N21" s="33" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N21" s="48"/>
+    </row>
+    <row customHeight="1" ht="34.5" r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>18</v>
       </c>
@@ -3235,43 +4423,48 @@
         <v>47</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="D22" s="35" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="E22" s="35" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="F22" s="36" t="s">
         <v>22</v>
       </c>
       <c r="G22" s="34" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="H22" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
+        <v>33</v>
+      </c>
+      <c r="I22" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="K22" s="36" t="s">
+        <v>22</v>
+      </c>
       <c r="L22" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="M22" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="M22" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="N22" s="34" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N22" s="49"/>
+    </row>
+    <row customHeight="1" ht="33.75" r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
       <c r="B23" s="11" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N23" s="50"/>
+    </row>
+    <row customHeight="1" ht="25.5" r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="16"/>
       <c r="B24" s="21"/>
       <c r="C24" s="40"/>
@@ -3285,17 +4478,156 @@
       <c r="K24" s="40"/>
       <c r="L24" s="40"/>
       <c r="M24" s="40"/>
-      <c r="N24" s="40"/>
+      <c r="N24" s="51"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N25" s="50"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N26" s="50"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N27" s="50"/>
+    </row>
+    <row ht="15.75" r="28" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N28" s="50"/>
+    </row>
+    <row ht="15.75" r="29" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="22"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
+      <c r="K29" s="44"/>
+      <c r="L29" s="45"/>
+      <c r="M29" s="32"/>
+      <c r="N29" s="48"/>
+    </row>
+    <row ht="38.25" r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="L30" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="M30" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="N30" s="50"/>
+    </row>
+    <row customHeight="1" ht="34.5" r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="F31" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="G31" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="H31" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="I31" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="J31" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="K31" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="L31" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="M31" s="36" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="33.75" r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="15"/>
+      <c r="B32" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="25.5" r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="16"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="40"/>
+      <c r="H33" s="40"/>
+      <c r="I33" s="40"/>
+      <c r="J33" s="40"/>
+      <c r="K33" s="40"/>
+      <c r="L33" s="40"/>
+      <c r="M33" s="40"/>
+      <c r="N33" s="46"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="F29:L29"/>
     <mergeCell ref="F2:L2"/>
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="F11:L11"/>
     <mergeCell ref="C20:E20"/>
     <mergeCell ref="F20:L20"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
committing to local machine
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/TestOutPutResultFolder/201819 Payroll Court order and Student Loan Test result.xlsx
+++ b/Salesforce_Core_Framework/TestOutPutResultFolder/201819 Payroll Court order and Student Loan Test result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Court Order and Student Loan Project\input sheet for scenario 1\Test Result output excel file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="10_ncr:8100000_{5C115C1E-E7FC-4B64-8A7C-C9344DCACF0D}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33"/>
+  <xr:revisionPtr documentId="10_ncr:8100000_{0105D948-B271-4454-B556-E439955DA8EA}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33"/>
   <bookViews>
-    <workbookView activeTab="5" firstSheet="1" windowHeight="4035" windowWidth="14955" xWindow="0" xr2:uid="{7CD66A07-AC55-4110-B71A-2F0C233FAD1E}" yWindow="0"/>
+    <workbookView activeTab="6" firstSheet="2" windowHeight="4035" windowWidth="14955" xWindow="0" xr2:uid="{7CD66A07-AC55-4110-B71A-2F0C233FAD1E}" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="AEO1971civildebt" r:id="rId1" sheetId="1"/>
@@ -19,6 +19,7 @@
     <sheet name="PAEO1971Maintenance" r:id="rId4" sheetId="4"/>
     <sheet name="PAEO1971Fine" r:id="rId5" sheetId="5"/>
     <sheet name="PAEO2003Fine" r:id="rId6" sheetId="6"/>
+    <sheet name="CTAEOCouncil tax" r:id="rId7" sheetId="7"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="89">
   <si>
     <t>Scenario Name</t>
   </si>
@@ -266,37 +267,37 @@
     <t>GBP 42.00</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
     <t>31/12/2018</t>
   </si>
   <si>
     <t>GBP 558.00</t>
+  </si>
+  <si>
+    <t>GBP 272.00</t>
+  </si>
+  <si>
+    <t>GBP 1,328.00</t>
+  </si>
+  <si>
+    <t>GBP 30.00</t>
+  </si>
+  <si>
+    <t>GBP 570.00</t>
+  </si>
+  <si>
+    <t>England C</t>
+  </si>
+  <si>
+    <t>CTAEOCouncil tax</t>
+  </si>
+  <si>
+    <t>DO NOT TOUCH AUTOMATION EMP 114</t>
+  </si>
+  <si>
+    <t>GBP 728.00</t>
+  </si>
+  <si>
+    <t>GBP 970.00</t>
   </si>
 </sst>
 </file>
@@ -603,7 +604,7 @@
       <color indexed="8"/>
     </font>
   </fonts>
-  <fills count="129">
+  <fills count="130">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -759,6 +760,11 @@
     <fill>
       <patternFill patternType="lightGray">
         <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor indexed="51"/>
       </patternFill>
     </fill>
     <fill>
@@ -1329,7 +1335,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="131">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1469,6 +1475,7 @@
     <xf applyFill="1" applyFont="1" borderId="0" fillId="27" fontId="20" numFmtId="0" xfId="0"/>
     <xf applyFill="1" applyFont="1" borderId="0" fillId="28" fontId="21" numFmtId="0" xfId="0"/>
     <xf applyFill="1" applyFont="1" borderId="0" fillId="29" fontId="22" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="30" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="4" fillId="4" fontId="4" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1478,72 +1485,72 @@
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="5" fillId="5" fontId="4" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="31" fontId="23" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="32" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="34" fontId="24" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="35" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="37" fontId="25" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="38" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="40" fontId="26" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="41" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="43" fontId="27" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="44" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="46" fontId="28" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="47" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="49" fontId="29" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="50" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="52" fontId="30" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="53" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="55" fontId="31" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="56" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="58" fontId="32" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="59" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="61" fontId="33" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="62" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="64" fontId="34" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="65" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="67" fontId="35" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="68" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="70" fontId="36" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="71" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="73" fontId="37" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="74" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="76" fontId="38" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="77" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="79" fontId="39" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="80" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="82" fontId="40" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="83" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="85" fontId="41" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="86" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="88" fontId="42" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="89" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="91" fontId="43" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="92" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="94" fontId="44" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="95" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="97" fontId="45" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="98" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="100" fontId="46" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="101" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="103" fontId="47" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="104" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="106" fontId="48" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="107" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="109" fontId="49" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="110" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="112" fontId="50" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="113" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="115" fontId="51" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="116" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="118" fontId="52" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="119" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="121" fontId="53" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="122" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="124" fontId="54" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="125" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="55" fillId="127" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="128" borderId="0" xfId="0" applyFill="true"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="32" fontId="23" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="33" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="35" fontId="24" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="36" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="38" fontId="25" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="39" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="41" fontId="26" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="42" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="44" fontId="27" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="45" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="47" fontId="28" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="48" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="50" fontId="29" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="51" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="53" fontId="30" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="54" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="56" fontId="31" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="57" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="59" fontId="32" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="60" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="62" fontId="33" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="63" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="65" fontId="34" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="66" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="68" fontId="35" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="69" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="71" fontId="36" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="72" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="74" fontId="37" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="75" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="77" fontId="38" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="78" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="80" fontId="39" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="81" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="83" fontId="40" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="84" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="86" fontId="41" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="87" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="89" fontId="42" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="90" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="92" fontId="43" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="93" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="95" fontId="44" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="96" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="98" fontId="45" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="99" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="101" fontId="46" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="102" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="104" fontId="47" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="105" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="107" fontId="48" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="108" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="110" fontId="49" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="111" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="113" fontId="50" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="114" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="116" fontId="51" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="117" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="119" fontId="52" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="120" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="122" fontId="53" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="123" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="125" fontId="54" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="126" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="55" fillId="128" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="129" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -1908,19 +1915,19 @@
         <v>29</v>
       </c>
       <c r="B2" s="19"/>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="62" t="s">
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="64"/>
       <c r="L2" s="20" t="s">
         <v>4</v>
       </c>
@@ -2106,19 +2113,19 @@
         <v>30</v>
       </c>
       <c r="B11" s="19"/>
-      <c r="C11" s="61" t="s">
+      <c r="C11" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="62" t="s">
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="I11" s="62"/>
-      <c r="J11" s="62"/>
-      <c r="K11" s="63"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="64"/>
       <c r="L11" s="20" t="s">
         <v>4</v>
       </c>
@@ -2362,19 +2369,19 @@
         <v>29</v>
       </c>
       <c r="B2" s="19"/>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="62" t="s">
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="64"/>
       <c r="L2" s="20" t="s">
         <v>4</v>
       </c>
@@ -2555,19 +2562,19 @@
         <v>30</v>
       </c>
       <c r="B11" s="19"/>
-      <c r="C11" s="61" t="s">
+      <c r="C11" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="62" t="s">
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="I11" s="62"/>
-      <c r="J11" s="62"/>
-      <c r="K11" s="63"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="64"/>
       <c r="L11" s="20" t="s">
         <v>4</v>
       </c>
@@ -2809,19 +2816,19 @@
         <v>29</v>
       </c>
       <c r="B2" s="19"/>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="62" t="s">
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="64"/>
       <c r="L2" s="20" t="s">
         <v>4</v>
       </c>
@@ -3002,19 +3009,19 @@
         <v>30</v>
       </c>
       <c r="B11" s="19"/>
-      <c r="C11" s="61" t="s">
+      <c r="C11" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="62" t="s">
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="I11" s="62"/>
-      <c r="J11" s="62"/>
-      <c r="K11" s="63"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="64"/>
       <c r="L11" s="20" t="s">
         <v>4</v>
       </c>
@@ -3252,12 +3259,12 @@
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
       <c r="E2" s="30"/>
-      <c r="F2" s="62" t="s">
+      <c r="F2" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
       <c r="J2" s="20" t="s">
         <v>4</v>
       </c>
@@ -3409,15 +3416,15 @@
         <v>30</v>
       </c>
       <c r="B11" s="22"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="62" t="s">
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="62"/>
-      <c r="H11" s="62"/>
-      <c r="I11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="64"/>
       <c r="J11" s="20" t="s">
         <v>4</v>
       </c>
@@ -3565,15 +3572,15 @@
         <v>43</v>
       </c>
       <c r="B20" s="22"/>
-      <c r="C20" s="61"/>
-      <c r="D20" s="61"/>
-      <c r="E20" s="61"/>
-      <c r="F20" s="62" t="s">
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G20" s="62"/>
-      <c r="H20" s="62"/>
-      <c r="I20" s="63"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="64"/>
       <c r="J20" s="20" t="s">
         <v>4</v>
       </c>
@@ -3781,15 +3788,15 @@
       <c r="C2" s="38"/>
       <c r="D2" s="38"/>
       <c r="E2" s="38"/>
-      <c r="F2" s="62" t="s">
+      <c r="F2" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="64"/>
       <c r="M2" s="20" t="s">
         <v>4</v>
       </c>
@@ -3977,18 +3984,18 @@
         <v>30</v>
       </c>
       <c r="B11" s="22"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="62" t="s">
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="62"/>
-      <c r="H11" s="62"/>
-      <c r="I11" s="62"/>
-      <c r="J11" s="62"/>
-      <c r="K11" s="62"/>
-      <c r="L11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="63"/>
+      <c r="L11" s="64"/>
       <c r="M11" s="20" t="s">
         <v>4</v>
       </c>
@@ -4172,18 +4179,18 @@
         <v>43</v>
       </c>
       <c r="B20" s="22"/>
-      <c r="C20" s="61"/>
-      <c r="D20" s="61"/>
-      <c r="E20" s="61"/>
-      <c r="F20" s="62" t="s">
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G20" s="62"/>
-      <c r="H20" s="62"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="62"/>
-      <c r="K20" s="62"/>
-      <c r="L20" s="63"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="63"/>
+      <c r="J20" s="63"/>
+      <c r="K20" s="63"/>
+      <c r="L20" s="64"/>
       <c r="M20" s="32"/>
       <c r="N20" s="44"/>
     </row>
@@ -4366,18 +4373,18 @@
         <v>52</v>
       </c>
       <c r="B29" s="22"/>
-      <c r="C29" s="61"/>
-      <c r="D29" s="61"/>
-      <c r="E29" s="61"/>
-      <c r="F29" s="62" t="s">
+      <c r="C29" s="62"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G29" s="62"/>
-      <c r="H29" s="62"/>
-      <c r="I29" s="62"/>
-      <c r="J29" s="62"/>
-      <c r="K29" s="62"/>
-      <c r="L29" s="63"/>
+      <c r="G29" s="63"/>
+      <c r="H29" s="63"/>
+      <c r="I29" s="63"/>
+      <c r="J29" s="63"/>
+      <c r="K29" s="63"/>
+      <c r="L29" s="64"/>
       <c r="M29" s="32"/>
       <c r="N29" s="44"/>
     </row>
@@ -4560,8 +4567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B79FD0B3-1F2E-476D-89A3-1D2D31F0C4E0}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4601,15 +4608,15 @@
         <v>29</v>
       </c>
       <c r="B2" s="19"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="62" t="s">
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
       <c r="J2" s="20" t="s">
         <v>69</v>
       </c>
@@ -4719,63 +4726,42 @@
         <v>28</v>
       </c>
       <c r="B6" s="21"/>
-      <c r="C6" s="80" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="80" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="80" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="80" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="80" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="80" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="80" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" s="80" t="s">
+      <c r="C6" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="58" t="s">
         <v>38</v>
       </c>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="56" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="D7" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="E7" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="F7" s="56" t="s">
-        <v>83</v>
-      </c>
-      <c r="G7" s="56" t="s">
-        <v>84</v>
-      </c>
-      <c r="H7" s="56" t="s">
-        <v>85</v>
-      </c>
-      <c r="I7" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="J7">
-        <v>9</v>
-      </c>
+      <c r="A7" s="56"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="56"/>
       <c r="K7" s="18"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -4813,15 +4799,15 @@
         <v>30</v>
       </c>
       <c r="B11" s="19"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="62" t="s">
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="62"/>
-      <c r="H11" s="62"/>
-      <c r="I11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="64"/>
       <c r="J11" s="20" t="s">
         <v>69</v>
       </c>
@@ -4927,28 +4913,28 @@
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="21"/>
-      <c r="C15" s="104" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="104" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="104" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="104" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" s="104" t="s">
-        <v>38</v>
-      </c>
-      <c r="H15" s="104" t="s">
-        <v>38</v>
-      </c>
-      <c r="I15" s="104" t="s">
-        <v>38</v>
-      </c>
-      <c r="J15" s="104" t="s">
+      <c r="C15" s="59" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="59" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="59" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="59" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="59" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="59" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="59" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" s="59" t="s">
         <v>38</v>
       </c>
       <c r="K15" s="18"/>
@@ -5010,15 +4996,15 @@
         <v>43</v>
       </c>
       <c r="B20" s="19"/>
-      <c r="C20" s="61"/>
-      <c r="D20" s="61"/>
-      <c r="E20" s="61"/>
-      <c r="F20" s="62" t="s">
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G20" s="62"/>
-      <c r="H20" s="62"/>
-      <c r="I20" s="63"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="64"/>
       <c r="J20" s="20" t="s">
         <v>69</v>
       </c>
@@ -5091,7 +5077,7 @@
         <v>75</v>
       </c>
       <c r="K22" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row ht="24" r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -5105,7 +5091,7 @@
         <v>77</v>
       </c>
       <c r="D23" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E23" t="s">
         <v>72</v>
@@ -5134,31 +5120,31 @@
         <v>28</v>
       </c>
       <c r="B24" s="21"/>
-      <c r="C24" t="s" s="129">
+      <c r="C24" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="D24" t="s" s="129">
+      <c r="D24" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="E24" t="s" s="128">
-        <v>38</v>
-      </c>
-      <c r="F24" t="s" s="128">
-        <v>38</v>
-      </c>
-      <c r="G24" t="s" s="128">
-        <v>38</v>
-      </c>
-      <c r="H24" t="s" s="128">
-        <v>38</v>
-      </c>
-      <c r="I24" t="s" s="129">
+      <c r="E24" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="G24" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="H24" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="I24" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="J24" t="s" s="129">
+      <c r="J24" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="K24" t="s" s="129">
+      <c r="K24" s="61" t="s">
         <v>65</v>
       </c>
     </row>
@@ -5226,4 +5212,598 @@
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3732E8F8-10C6-4AF8-BF9C-4562F78A0ED3}">
+  <dimension ref="A1:J27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="19.5703125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="30.75" r="1" spans="1:10" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row ht="26.25" r="2" spans="1:10" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="48" r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="30.75" r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="57" t="s">
+        <v>64</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="30" r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="26.25" r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="81" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="81" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="81" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="81" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="81" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="81" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="81" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="81" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="56"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="56"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J8" s="18"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+    </row>
+    <row ht="15.75" r="10" spans="1:10" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+    </row>
+    <row ht="39" r="11" spans="1:10" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="19"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="64"/>
+      <c r="J11" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="45.75" r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="26.25" r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="33.75" r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="11"/>
+      <c r="C14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" t="s">
+        <v>64</v>
+      </c>
+      <c r="I14" t="s">
+        <v>80</v>
+      </c>
+      <c r="J14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="24.75" r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="105" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="106" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="105" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="105" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="105" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="105" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="105" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" s="105" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+    </row>
+    <row ht="15.75" r="19" spans="1:10" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+    </row>
+    <row ht="26.25" r="20" spans="1:10" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="19"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="63"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="64"/>
+      <c r="J20" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="45.75" r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="34.5" r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="J22" s="13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="30.75" r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="11"/>
+      <c r="C23" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" t="s">
+        <v>84</v>
+      </c>
+      <c r="F23" t="s">
+        <v>82</v>
+      </c>
+      <c r="G23" t="s">
+        <v>58</v>
+      </c>
+      <c r="H23" t="s">
+        <v>64</v>
+      </c>
+      <c r="I23" t="s">
+        <v>82</v>
+      </c>
+      <c r="J23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="26.25" r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="21"/>
+      <c r="C24" t="s" s="129">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s" s="130">
+        <v>65</v>
+      </c>
+      <c r="E24" t="s" s="129">
+        <v>38</v>
+      </c>
+      <c r="F24" t="s" s="129">
+        <v>38</v>
+      </c>
+      <c r="G24" t="s" s="129">
+        <v>38</v>
+      </c>
+      <c r="H24" t="s" s="129">
+        <v>38</v>
+      </c>
+      <c r="I24" t="s" s="129">
+        <v>38</v>
+      </c>
+      <c r="J24" t="s" s="129">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="F20:I20"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>